<commit_message>
Volume adjust, 2minutes remind, Plus minus void
</commit_message>
<xml_diff>
--- a/Audio_Update/Audio.xlsx
+++ b/Audio_Update/Audio.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\Audio_Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RunningMachine\Audio_Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FCFC65-CC90-4B1C-88F9-1736D0BB96D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -133,36 +132,12 @@
     <t>Cài đặt độ dốc 9%</t>
   </si>
   <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ 1km trên giờ, hãy bấm phím speed + để tăng tốc độ lên 2km trên giờ</t>
-  </si>
-  <si>
     <t>021</t>
   </si>
   <si>
     <t>022</t>
   </si>
   <si>
-    <t>023</t>
-  </si>
-  <si>
-    <t>024</t>
-  </si>
-  <si>
-    <t>025</t>
-  </si>
-  <si>
-    <t>026</t>
-  </si>
-  <si>
-    <t>027</t>
-  </si>
-  <si>
-    <t>Hãy nhấn phím Stop để kết thúc buổi tập.</t>
-  </si>
-  <si>
-    <t>028</t>
-  </si>
-  <si>
     <t>Cài đặt độ dài quãng đường chạy. Nhấn phím cộng để tăng, Nhấn phím trừ để giảm quãng đường chạy, đơn vị là trăm mét. Nhấn phím Mode lần nữa để chuyển sang cài đặt lượng năng lượng tiêu thụ. Nhấn phím start để bắt đầu chạy với các thông số mà bạn đã cài đặt. Nhấn phím Stop để quay trở lại.</t>
   </si>
   <si>
@@ -181,38 +156,28 @@
     <t>Bạn đã tắt trợ lý ảo</t>
   </si>
   <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ 2km trên giờ, hãy bấm phím speed + để tăng tốc độ lên 4km trên giờ</t>
-  </si>
-  <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ 4km trên giờ, hãy bấm phím speed + để tăng tốc độ lên 6km trên giờ</t>
-  </si>
-  <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ 6km trên giờ, hãy bấm phím speed + để tăng tốc độ lên 8km trên giờ</t>
-  </si>
-  <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ 8km trên giờ, hãy bấm phím speed trừ để giảm tốc độ xuống 6km trên giờ</t>
-  </si>
-  <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ 6km trên giờ, hãy bấm phím speed trừ để giảm tốc độ xuống 4km trên giờ</t>
-  </si>
-  <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ 4km trên giờ, hãy bấm phím speed trừ để giảm tốc độ xuống 2km trên giờ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bạn đã chạy được 2 phút với tốc độ 2km trên giờ, hãy bấm phím speed trừ để giảm tốc độ xuống 1km trên giờ. Bạn hãy đi bộ 2 phút trước khi kết thúc buổi tập nhé
-</t>
-  </si>
-  <si>
     <t>Bạn đã đi giày và khởi động chưa, nếu chưa hãy nhấn phím stop sau đó lựa chọn bài tập gập bụng, xoay eo đã tích hợp trên máy</t>
   </si>
   <si>
     <t>Volume sound</t>
+  </si>
+  <si>
+    <t>Bạn đã chạy được 2 phút với tốc độ hiện tại, hãy bấm phím speed cộng để tăng hoặc speed trừ để giảm tốc độ.</t>
+  </si>
+  <si>
+    <t>Sleep mode 10p</t>
+  </si>
+  <si>
+    <t>Tăng tốc độ, chú ý giữ an toàn nhé</t>
+  </si>
+  <si>
+    <t>Giảm tốc độ, chú ý giữ an toàn nhé</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,22 +507,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="87.81640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -579,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -590,7 +555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -601,7 +566,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -612,7 +577,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -623,7 +588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -634,7 +599,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -642,10 +607,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -656,7 +621,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -664,10 +629,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -678,7 +643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -689,7 +654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -700,7 +665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -711,7 +676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -719,10 +684,10 @@
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -730,10 +695,10 @@
         <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -741,10 +706,10 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -752,10 +717,10 @@
         <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -763,10 +728,10 @@
         <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -774,10 +739,10 @@
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -785,185 +750,140 @@
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="4"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B52" s="4"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B56" s="3"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B58" s="3"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for incline button
</commit_message>
<xml_diff>
--- a/Audio_Update/Audio.xlsx
+++ b/Audio_Update/Audio.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RunningMachine\Audio_Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\Audio_Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A80BCF-316D-4877-B1D4-6EFBE48608F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -129,9 +130,6 @@
   </si>
   <si>
     <t>Bạn đã tắt trợ lý ảo</t>
-  </si>
-  <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ hiện tại, hãy bấm phím speed cộng để tăng hoặc speed trừ để giảm tốc độ.</t>
   </si>
   <si>
     <t>Tăng tốc độ, chú ý giữ an toàn nhé</t>
@@ -179,15 +177,33 @@
   <si>
     <t>Cài đặt mức năng lương tiêu thụ. Nhấn phím cộng để tăng, nhấn phím trừ để giảm mức năng lượng tiêu thụ. Đơn vị là kalo. Nhấn phím start để bắt đầu chạy với các thông số mà bạn đã cài đặt. Nhấn phím Stốp hoặc Mode lần nữa để quay trở lại.</t>
   </si>
+  <si>
+    <t>Bạn đã chạy được 2 phút với tốc độ và độ dốc hiện tại, hãy bấm phím speed cộng để tăng hoặc speed trừ để giảm tốc độ, bấm phím incline cộng để tăng hoặc incline trừ để giảm độ dốc</t>
+  </si>
+  <si>
+    <t>Tăng độ dốc, chú ý giữ an toàn nhé</t>
+  </si>
+  <si>
+    <t>Giảm độ dốc, chú ý giữ an toàn nhé</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -513,22 +529,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.453125" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="87.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -547,10 +563,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -561,7 +577,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -569,10 +585,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -583,7 +599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -591,10 +607,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -602,10 +618,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -613,10 +629,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -624,10 +640,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -635,10 +651,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -646,10 +662,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -660,7 +676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -671,7 +687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -682,7 +698,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -693,7 +709,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -704,7 +720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -715,7 +731,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -726,7 +742,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -737,7 +753,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -745,10 +761,10 @@
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -756,10 +772,10 @@
         <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -767,10 +783,10 @@
         <v>28</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -778,131 +794,142 @@
         <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Change Pin for SafeKey
</commit_message>
<xml_diff>
--- a/Audio_Update/Audio.xlsx
+++ b/Audio_Update/Audio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\Audio_Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FC7BFC-4FAD-4A8C-B2B1-F11B843FC663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A4B845-DEC7-454C-A8DF-9E3F27E37EB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -157,43 +157,55 @@
   </si>
   <si>
     <t>Bài tập 1:  Tốc độ chạy thấp nhất, Nhấn phím Start để bắt đầu chạy. Nhấn phím Program để chuyển sang chế độ khác. Nhấn phím stốp để dừng lại.</t>
+  </si>
+  <si>
+    <t>Bạn đã đi giày và khởi động chưa, nếu chưa hãy nhấn phím stốp sau đó lựa chọn bài tập gập bụng, xoay eo đã tích hợp trên máy</t>
+  </si>
+  <si>
+    <t>Cài đặt thời gian chạy, Nhấn phím cộng để tăng nhấn phím trừ để giảm thời gian chạy. Đơn vị là phút. Nhấn phím Mode lần nữa để chuyển sang cài đặt quãng đường chạy. Nhấn phím start để bắt đầu chạy với các thông số mà bạn đã cài đặt. Nhấn phím Stốp để quay trở lại.</t>
+  </si>
+  <si>
+    <t>Cài đặt độ dài quãng đường chạy. Nhấn phím cộng để tăng, Nhấn phím trừ để giảm quãng đường chạy, đơn vị là trăm mét. Nhấn phím Mode lần nữa để chuyển sang cài đặt lượng năng lượng tiêu thụ. Nhấn phím start để bắt đầu chạy với các thông số mà bạn đã cài đặt. Nhấn phím Stốp để quay trở lại.</t>
+  </si>
+  <si>
+    <t>Cài đặt mức năng lương tiêu thụ. Nhấn phím cộng để tăng, nhấn phím trừ để giảm mức năng lượng tiêu thụ. Đơn vị là kalo. Nhấn phím start để bắt đầu chạy với các thông số mà bạn đã cài đặt. Nhấn phím Stốp hoặc Mode lần nữa để quay trở lại.</t>
+  </si>
+  <si>
+    <t>Bạn đã chạy được 2 phút với tốc độ và độ dốc hiện tại, hãy bấm phím speed cộng để tăng hoặc speed trừ để giảm tốc độ, bấm phím incline cộng để tăng hoặc incline trừ để giảm độ dốc</t>
+  </si>
+  <si>
+    <t>Tăng độ dốc, chú ý giữ an toàn nhé</t>
+  </si>
+  <si>
+    <t>Giảm độ dốc, chú ý giữ an toàn nhé</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>Bạn hãy cài khóa an toàn trước khi luyện tập nhé</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Thêm lời nhắc cài khóa an toàn</t>
+  </si>
+  <si>
+    <t>Thêm lời khen sau 20p</t>
+  </si>
+  <si>
+    <t>Mát xa bằng thiết bị tích hợp trên máy</t>
   </si>
   <si>
     <t>Chào mừng bạn đến với máy chạy Sport One.
 Nhấn phím start để chạy với tốc độ mặc định.
 Nhấn phím Stốp để dừng lại, hoặc quay trở lại cài đặt ban đầu.
 Nhấn phím Program để lựa chọn chế độ thích hợp. 
-Nhấn phím Mode để cài đặt thêm các thông số khác như tốc độ chạy, thời gian, quãng đường, lượng calo tiêu thụ.</t>
-  </si>
-  <si>
-    <t>Bạn đã đi giày và khởi động chưa, nếu chưa hãy nhấn phím stốp sau đó lựa chọn bài tập gập bụng, xoay eo đã tích hợp trên máy</t>
-  </si>
-  <si>
-    <t>Cài đặt thời gian chạy, Nhấn phím cộng để tăng nhấn phím trừ để giảm thời gian chạy. Đơn vị là phút. Nhấn phím Mode lần nữa để chuyển sang cài đặt quãng đường chạy. Nhấn phím start để bắt đầu chạy với các thông số mà bạn đã cài đặt. Nhấn phím Stốp để quay trở lại.</t>
-  </si>
-  <si>
-    <t>Cài đặt độ dài quãng đường chạy. Nhấn phím cộng để tăng, Nhấn phím trừ để giảm quãng đường chạy, đơn vị là trăm mét. Nhấn phím Mode lần nữa để chuyển sang cài đặt lượng năng lượng tiêu thụ. Nhấn phím start để bắt đầu chạy với các thông số mà bạn đã cài đặt. Nhấn phím Stốp để quay trở lại.</t>
-  </si>
-  <si>
-    <t>Cài đặt mức năng lương tiêu thụ. Nhấn phím cộng để tăng, nhấn phím trừ để giảm mức năng lượng tiêu thụ. Đơn vị là kalo. Nhấn phím start để bắt đầu chạy với các thông số mà bạn đã cài đặt. Nhấn phím Stốp hoặc Mode lần nữa để quay trở lại.</t>
-  </si>
-  <si>
-    <t>Bạn đã chạy được 2 phút với tốc độ và độ dốc hiện tại, hãy bấm phím speed cộng để tăng hoặc speed trừ để giảm tốc độ, bấm phím incline cộng để tăng hoặc incline trừ để giảm độ dốc</t>
-  </si>
-  <si>
-    <t>Tăng độ dốc, chú ý giữ an toàn nhé</t>
-  </si>
-  <si>
-    <t>Giảm độ dốc, chú ý giữ an toàn nhé</t>
-  </si>
-  <si>
-    <t>025</t>
-  </si>
-  <si>
-    <t>026</t>
-  </si>
-  <si>
-    <t>Bạn hãy cài khóa an toàn trước khi luyện tập nhé</t>
+Nhấn phím Mode để cài đặt thêm các thông số khác như thời gian, quãng đường, lượng calo tiêu thụ.</t>
   </si>
 </sst>
 </file>
@@ -536,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,9 +560,11 @@
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="87.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,8 +574,11 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -569,10 +586,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -582,8 +605,11 @@
       <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -594,7 +620,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -605,7 +631,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -616,7 +642,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -627,7 +653,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -635,10 +661,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -646,10 +672,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -657,10 +683,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -668,10 +694,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -682,7 +708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -693,7 +719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -704,7 +730,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -715,7 +741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -767,7 +793,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,7 +848,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,10 +856,10 @@
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,10 +867,10 @@
         <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>